<commit_message>
alteração no planejamento semanal
</commit_message>
<xml_diff>
--- a/Documentação/Planejamentos/Planejamento semanal.xlsx
+++ b/Documentação/Planejamentos/Planejamento semanal.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bruno\Desktop\Projeto_ProVagas\Planejamentos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bruno\Desktop\Projeto_ProVagas\Documentação\Planejamentos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E874B99-E6B2-4727-9B43-3A2E992C638B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F88635E9-48C4-4587-9C54-5DBD8262FC1E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="40">
   <si>
     <t>PLANEJAMENTO SEMANAL - CONTROLE CLASSROOM</t>
   </si>
@@ -115,9 +115,6 @@
     <t>Modelo Lógico</t>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
     <t xml:space="preserve">  </t>
   </si>
   <si>
@@ -133,13 +130,16 @@
     <t>DQL</t>
   </si>
   <si>
-    <t>Planejamento BD</t>
-  </si>
-  <si>
     <t>Mer - Modelo Entidade Relacionamento</t>
   </si>
   <si>
     <t xml:space="preserve">   </t>
+  </si>
+  <si>
+    <t>Cardinalidades</t>
+  </si>
+  <si>
+    <t>?</t>
   </si>
 </sst>
 </file>
@@ -331,6 +331,7 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -347,7 +348,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -568,8 +568,8 @@
   </sheetPr>
   <dimension ref="A1:T26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="M11" sqref="M11"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -578,50 +578,50 @@
     <col min="5" max="5" width="33.7109375" customWidth="1"/>
     <col min="9" max="9" width="15.85546875" customWidth="1"/>
     <col min="13" max="13" width="19.28515625" customWidth="1"/>
-    <col min="17" max="17" width="16.140625" customWidth="1"/>
+    <col min="17" max="17" width="19.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
-      <c r="H1" s="13"/>
-      <c r="I1" s="13"/>
-      <c r="J1" s="13"/>
-      <c r="K1" s="13"/>
-      <c r="L1" s="13"/>
-      <c r="M1" s="13"/>
-      <c r="N1" s="13"/>
-      <c r="O1" s="13"/>
-      <c r="P1" s="13"/>
-      <c r="Q1" s="13"/>
-      <c r="R1" s="13"/>
-      <c r="S1" s="13"/>
-      <c r="T1" s="14"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="14"/>
+      <c r="I1" s="14"/>
+      <c r="J1" s="14"/>
+      <c r="K1" s="14"/>
+      <c r="L1" s="14"/>
+      <c r="M1" s="14"/>
+      <c r="N1" s="14"/>
+      <c r="O1" s="14"/>
+      <c r="P1" s="14"/>
+      <c r="Q1" s="14"/>
+      <c r="R1" s="14"/>
+      <c r="S1" s="14"/>
+      <c r="T1" s="15"/>
     </row>
     <row r="2" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="17" t="s">
+      <c r="B2" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="13"/>
-      <c r="D2" s="14"/>
+      <c r="C2" s="14"/>
+      <c r="D2" s="15"/>
       <c r="E2" s="1" t="s">
         <v>3</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="18"/>
-      <c r="H2" s="19"/>
+      <c r="G2" s="19"/>
+      <c r="H2" s="20"/>
       <c r="I2" s="2"/>
       <c r="J2" s="2"/>
       <c r="K2" s="2"/>
@@ -636,64 +636,64 @@
       <c r="T2" s="3"/>
     </row>
     <row r="3" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A3" s="15" t="s">
+      <c r="A3" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="13"/>
-      <c r="C3" s="13"/>
-      <c r="D3" s="14"/>
-      <c r="E3" s="15" t="s">
+      <c r="B3" s="14"/>
+      <c r="C3" s="14"/>
+      <c r="D3" s="15"/>
+      <c r="E3" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="F3" s="13"/>
-      <c r="G3" s="13"/>
-      <c r="H3" s="14"/>
-      <c r="I3" s="15" t="s">
+      <c r="F3" s="14"/>
+      <c r="G3" s="14"/>
+      <c r="H3" s="15"/>
+      <c r="I3" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="J3" s="13"/>
-      <c r="K3" s="13"/>
-      <c r="L3" s="14"/>
-      <c r="M3" s="15" t="s">
+      <c r="J3" s="14"/>
+      <c r="K3" s="14"/>
+      <c r="L3" s="15"/>
+      <c r="M3" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="N3" s="13"/>
-      <c r="O3" s="13"/>
-      <c r="P3" s="14"/>
-      <c r="Q3" s="15" t="s">
+      <c r="N3" s="14"/>
+      <c r="O3" s="14"/>
+      <c r="P3" s="15"/>
+      <c r="Q3" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="R3" s="13"/>
-      <c r="S3" s="13"/>
-      <c r="T3" s="14"/>
+      <c r="R3" s="14"/>
+      <c r="S3" s="14"/>
+      <c r="T3" s="15"/>
     </row>
     <row r="4" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A4" s="16"/>
-      <c r="B4" s="13"/>
-      <c r="C4" s="13"/>
-      <c r="D4" s="14"/>
-      <c r="E4" s="16"/>
-      <c r="F4" s="13"/>
-      <c r="G4" s="13"/>
-      <c r="H4" s="14"/>
-      <c r="I4" s="16">
+      <c r="A4" s="17"/>
+      <c r="B4" s="14"/>
+      <c r="C4" s="14"/>
+      <c r="D4" s="15"/>
+      <c r="E4" s="17"/>
+      <c r="F4" s="14"/>
+      <c r="G4" s="14"/>
+      <c r="H4" s="15"/>
+      <c r="I4" s="17">
         <v>44020</v>
       </c>
-      <c r="J4" s="13"/>
-      <c r="K4" s="13"/>
-      <c r="L4" s="14"/>
-      <c r="M4" s="16">
+      <c r="J4" s="14"/>
+      <c r="K4" s="14"/>
+      <c r="L4" s="15"/>
+      <c r="M4" s="17">
         <v>44021</v>
       </c>
-      <c r="N4" s="13"/>
-      <c r="O4" s="13"/>
-      <c r="P4" s="14"/>
-      <c r="Q4" s="16">
+      <c r="N4" s="14"/>
+      <c r="O4" s="14"/>
+      <c r="P4" s="15"/>
+      <c r="Q4" s="17">
         <v>44022</v>
       </c>
-      <c r="R4" s="13"/>
-      <c r="S4" s="13"/>
-      <c r="T4" s="14"/>
+      <c r="R4" s="14"/>
+      <c r="S4" s="14"/>
+      <c r="T4" s="15"/>
     </row>
     <row r="5" spans="1:20" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
@@ -866,19 +866,21 @@
       </c>
       <c r="G8" s="6"/>
       <c r="H8" s="3"/>
-      <c r="I8" s="11" t="s">
-        <v>30</v>
+      <c r="I8" s="12" t="s">
+        <v>32</v>
       </c>
       <c r="J8" s="7"/>
       <c r="K8" s="6"/>
       <c r="L8" s="3"/>
       <c r="M8" s="11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="N8" s="6"/>
       <c r="O8" s="6"/>
       <c r="P8" s="3"/>
-      <c r="Q8" s="11"/>
+      <c r="Q8" s="11" t="s">
+        <v>29</v>
+      </c>
       <c r="R8" s="11"/>
       <c r="S8" s="6"/>
       <c r="T8" s="3"/>
@@ -889,21 +891,21 @@
       <c r="C9" s="6"/>
       <c r="D9" s="3"/>
       <c r="E9" s="11" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="F9" s="11" t="s">
         <v>24</v>
       </c>
       <c r="G9" s="6"/>
       <c r="H9" s="3"/>
-      <c r="I9" s="3" t="s">
-        <v>34</v>
+      <c r="I9" s="11" t="s">
+        <v>30</v>
       </c>
       <c r="J9" s="6"/>
       <c r="K9" s="6"/>
       <c r="L9" s="3"/>
-      <c r="M9" s="11" t="s">
-        <v>36</v>
+      <c r="M9" s="3" t="s">
+        <v>33</v>
       </c>
       <c r="N9" s="6"/>
       <c r="O9" s="6"/>
@@ -919,21 +921,19 @@
       <c r="C10" s="6"/>
       <c r="D10" s="3"/>
       <c r="E10" s="11" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F10" s="11" t="s">
-        <v>24</v>
+        <v>39</v>
       </c>
       <c r="G10" s="6"/>
       <c r="H10" s="3"/>
-      <c r="I10" s="3" t="s">
-        <v>35</v>
-      </c>
+      <c r="I10" s="3"/>
       <c r="J10" s="6"/>
       <c r="K10" s="6"/>
       <c r="L10" s="3"/>
-      <c r="M10" s="11" t="s">
-        <v>28</v>
+      <c r="M10" s="3" t="s">
+        <v>34</v>
       </c>
       <c r="N10" s="11"/>
       <c r="O10" s="6"/>
@@ -952,13 +952,13 @@
       <c r="F11" s="6"/>
       <c r="G11" s="6"/>
       <c r="H11" s="3"/>
-      <c r="I11" s="20" t="s">
-        <v>33</v>
-      </c>
+      <c r="I11" s="11"/>
       <c r="J11" s="11"/>
       <c r="K11" s="6"/>
       <c r="L11" s="3"/>
-      <c r="M11" s="11"/>
+      <c r="M11" s="11" t="s">
+        <v>35</v>
+      </c>
       <c r="N11" s="11"/>
       <c r="O11" s="6"/>
       <c r="P11" s="3"/>
@@ -976,15 +976,13 @@
       <c r="F12" s="6"/>
       <c r="G12" s="6"/>
       <c r="H12" s="3"/>
-      <c r="I12" s="20" t="s">
-        <v>31</v>
-      </c>
+      <c r="I12" s="3"/>
       <c r="J12" s="11"/>
       <c r="K12" s="11" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="L12" s="3"/>
-      <c r="M12" s="6"/>
+      <c r="M12" s="11"/>
       <c r="N12" s="6"/>
       <c r="O12" s="6"/>
       <c r="P12" s="3"/>
@@ -998,15 +996,14 @@
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
-      <c r="E13" s="20"/>
+      <c r="E13" s="12"/>
       <c r="F13" s="3"/>
       <c r="G13" s="3"/>
       <c r="H13" s="3"/>
-      <c r="I13" s="6"/>
+      <c r="I13" s="3"/>
       <c r="J13" s="6"/>
       <c r="K13" s="6"/>
       <c r="L13" s="3"/>
-      <c r="M13" s="7"/>
       <c r="N13" s="7"/>
       <c r="O13" s="7"/>
       <c r="P13" s="3"/>
@@ -1065,7 +1062,7 @@
         <v>15</v>
       </c>
       <c r="H17" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">

</xml_diff>